<commit_message>
added naive baseline that analyzes measures independently
</commit_message>
<xml_diff>
--- a/models/sft/pcs/properties.xlsx
+++ b/models/sft/pcs/properties.xlsx
@@ -342,7 +342,7 @@
   <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q4:Q5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -354,127 +354,127 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0.7</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>1.1000000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1.3</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1.4</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>1.7</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>1.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1.9</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2.1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2.2000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>2.2999999999999998</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>